<commit_message>
[🛠️Fix] Table road fix
- json 배열 바깥쪽에 변환 후 담을 리스트 이름 매칭시킨 후 담도록 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E8CB39-5E94-40FC-A457-56E01187DCD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB86F81-925D-4915-8E99-542765CB9617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="825" windowWidth="17205" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Data\SummonTable\EquipmentSummonTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,10 @@
   </si>
   <si>
     <t>Probability : Int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SummonGrade : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -99,11 +103,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:B8" totalsRowShown="0">
-  <autoFilter ref="A2:B8" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="ItemId : Int"/>
-    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="Probability : Int"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:C14" totalsRowShown="0">
+  <autoFilter ref="A2:C14" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="SummonGrade : Int"/>
+    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : Int"/>
+    <tableColumn id="3" xr3:uid="{6233F03A-7423-45FA-8858-E7CF6806ED7B}" name="Probability : Int"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -372,77 +377,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>10001</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
+        <f>A3</f>
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>10002</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
+        <f t="shared" ref="A5:A8" si="0">A4</f>
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>10003</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>10005</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>10006</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>10007</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>50</v>
+      </c>
+      <c r="D8">
+        <f>SUM(C3:C8)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>B3</f>
+        <v>10001</v>
+      </c>
+      <c r="C9">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>A9</f>
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ref="B10:B14" si="1">B4</f>
+        <v>10002</v>
+      </c>
+      <c r="C10">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" ref="A11:A14" si="2">A10</f>
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>10003</v>
+      </c>
+      <c r="C11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>10005</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>10006</v>
+      </c>
+      <c r="C13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>10007</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <f>SUM(C9:C14)</f>
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[➕Add] Summon Level process Apply
- 확률 테이블 로드 시 중복되는 확률 있으면 문제 있던 부분 수정
- 뽑기 시 뽑기 레벨이 변경되면 확률 변경되게 적용
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB86F81-925D-4915-8E99-542765CB9617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA67C7F-C437-4EF1-BA15-C15700DECAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,8 +103,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:C14" totalsRowShown="0">
-  <autoFilter ref="A2:C14" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:C32" totalsRowShown="0">
+  <autoFilter ref="A2:C32" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : Int"/>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
         <v>10001</v>
       </c>
       <c r="C3">
-        <v>5000</v>
+        <v>9995</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -426,7 +426,7 @@
         <v>10002</v>
       </c>
       <c r="C4">
-        <v>2500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -438,7 +438,7 @@
         <v>10003</v>
       </c>
       <c r="C5">
-        <v>1500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -450,7 +450,7 @@
         <v>10005</v>
       </c>
       <c r="C6">
-        <v>700</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -462,7 +462,7 @@
         <v>10006</v>
       </c>
       <c r="C7">
-        <v>250</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -474,7 +474,7 @@
         <v>10007</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>SUM(C3:C8)</f>
@@ -490,7 +490,7 @@
         <v>10001</v>
       </c>
       <c r="C9">
-        <v>3500</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -499,11 +499,11 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B14" si="1">B4</f>
+        <f t="shared" ref="B10:B32" si="1">B4</f>
         <v>10002</v>
       </c>
       <c r="C10">
-        <v>3000</v>
+        <v>9995</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -516,7 +516,7 @@
         <v>10003</v>
       </c>
       <c r="C11">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>10005</v>
       </c>
       <c r="C12">
-        <v>1000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>10006</v>
       </c>
       <c r="C13">
-        <v>400</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -555,11 +555,242 @@
         <v>10007</v>
       </c>
       <c r="C14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f>SUM(C9:C14)</f>
         <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f>B9</f>
+        <v>10001</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>A15</f>
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>10002</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" ref="A17:A20" si="3">A16</f>
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>10003</v>
+      </c>
+      <c r="C17">
+        <v>9995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>10005</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>10006</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>10007</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <f>B15</f>
+        <v>10001</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>A21</f>
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>10002</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" ref="A23:A26" si="4">A22</f>
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>10003</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>10005</v>
+      </c>
+      <c r="C24">
+        <v>9995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>10006</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>10007</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <f>B21</f>
+        <v>10001</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f>A27</f>
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>10002</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" ref="A29:A32" si="5">A28</f>
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>10003</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>10005</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>10006</v>
+      </c>
+      <c r="C31">
+        <v>9995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>10007</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[🐛BugFix] Table change error fix
- 테이블 변수를 수정하지 않아 뽑기 레벨이 변경되어도 참조하는 테이블이 그대로여서 문제가 생겼던 부분 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA67C7F-C437-4EF1-BA15-C15700DECAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65DE636-409E-4D6F-AFD9-A022827010FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="1350" windowWidth="17205" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,8 +379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[🛠️Fix] Item probability fix
- 확률 테이블 임시 수정
- 방어구 등장 가능하도록 수정
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65DE636-409E-4D6F-AFD9-A022827010FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A34429-D182-412C-9317-B76EDEDFE23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8850" yWindow="1350" windowWidth="17205" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,8 +103,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:C32" totalsRowShown="0">
-  <autoFilter ref="A2:C32" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}" name="표1" displayName="표1" ref="A2:C62" totalsRowShown="0">
+  <autoFilter ref="A2:C62" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : Int"/>
@@ -377,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -414,7 +414,7 @@
         <v>10001</v>
       </c>
       <c r="C3">
-        <v>9995</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -431,7 +431,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A8" si="0">A4</f>
+        <f t="shared" ref="A5:A14" si="0">A4</f>
         <v>1</v>
       </c>
       <c r="B5">
@@ -476,44 +476,38 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <f>SUM(C3:C8)</f>
-        <v>10000</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B9">
-        <f>B3</f>
-        <v>10001</v>
+        <v>20001</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f>A9</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B10">
-        <f t="shared" ref="B10:B32" si="1">B4</f>
-        <v>10002</v>
+        <v>20002</v>
       </c>
       <c r="C10">
-        <v>9995</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" ref="A11:A14" si="2">A10</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
-        <v>10003</v>
+        <v>20003</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -521,12 +515,11 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
-        <v>10005</v>
+        <v>20005</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -534,12 +527,11 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
-        <v>10006</v>
+        <v>20006</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -547,27 +539,26 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
-        <v>10007</v>
+        <v>20007</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <f>SUM(C9:C14)</f>
+        <f>SUM(C3:C14)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <f>B9</f>
+        <f t="shared" ref="B15:B20" si="1">B3</f>
         <v>10001</v>
       </c>
       <c r="C15">
@@ -577,33 +568,33 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>A15</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
         <v>10002</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" ref="A17:A20" si="3">A16</f>
-        <v>3</v>
+        <f t="shared" ref="A17:A20" si="2">A16</f>
+        <v>2</v>
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
         <v>10003</v>
       </c>
       <c r="C17">
-        <v>9995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
@@ -613,10 +604,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
@@ -626,10 +617,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
@@ -639,157 +630,540 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <f>B15</f>
-        <v>10001</v>
+        <v>20001</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>A21</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
-        <v>10002</v>
+        <v>20002</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" ref="A23:A26" si="4">A22</f>
-        <v>4</v>
+        <f t="shared" ref="A23:A26" si="3">A22</f>
+        <v>2</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
-        <v>10003</v>
+        <v>20003</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
-        <v>10005</v>
+        <v>20005</v>
       </c>
       <c r="C24">
-        <v>9995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
-        <v>10006</v>
+        <v>20006</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
-        <v>10007</v>
+        <v>20007</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>SUM(C15:C26)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <f>B21</f>
+        <f t="shared" ref="B27:B62" si="4">B15</f>
         <v>10001</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>A27</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10002</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" ref="A29:A32" si="5">A28</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10003</v>
       </c>
       <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10005</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10006</v>
       </c>
       <c r="C31">
-        <v>9995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="4"/>
+        <v>10007</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="4"/>
+        <v>20001</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>A33</f>
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="4"/>
+        <v>20002</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" ref="A35:A38" si="6">A34</f>
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="4"/>
+        <v>20003</v>
+      </c>
+      <c r="C35">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="4"/>
+        <v>20005</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="4"/>
+        <v>20006</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="4"/>
+        <v>20007</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="4"/>
+        <v>10001</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f>A39</f>
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="4"/>
+        <v>10002</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" ref="A41:A44" si="7">A40</f>
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="4"/>
+        <v>10003</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="4"/>
+        <v>10005</v>
+      </c>
+      <c r="C42">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="4"/>
+        <v>10006</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="4"/>
+        <v>10007</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="4"/>
+        <v>20001</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f>A45</f>
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="4"/>
+        <v>20002</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" ref="A47:A50" si="8">A46</f>
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="4"/>
+        <v>20003</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="4"/>
+        <v>20005</v>
+      </c>
+      <c r="C48">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="4"/>
+        <v>20006</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="4"/>
+        <v>20007</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>5</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="1"/>
+      <c r="B51">
+        <f t="shared" si="4"/>
+        <v>10001</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f>A51</f>
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="4"/>
+        <v>10002</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" ref="A53:A56" si="9">A52</f>
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="4"/>
+        <v>10003</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="4"/>
+        <v>10005</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="4"/>
+        <v>10006</v>
+      </c>
+      <c r="C55">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="4"/>
         <v>10007</v>
       </c>
-      <c r="C32">
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="4"/>
+        <v>20001</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f>A57</f>
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="4"/>
+        <v>20002</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" ref="A59:A62" si="10">A58</f>
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="4"/>
+        <v>20003</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="4"/>
+        <v>20005</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="4"/>
+        <v>20006</v>
+      </c>
+      <c r="C61">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="4"/>
+        <v>20007</v>
+      </c>
+      <c r="C62">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[🛠️Fix] Summon table and manager fix
- 아이템 Id가 string 형식으로 바뀌어서 그에 맞춰 테이블 및 매니저도 자료형 변경에 대응 작업
- 팝업은 일단 막아둠
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A34429-D182-412C-9317-B76EDEDFE23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC36D6-CC60-48A7-A1C5-F664094E03AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Data\SummonTable\EquipmentSummonTable.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ItemId : Int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SummonGrade : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ItemId : String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W0001</t>
+  </si>
+  <si>
+    <t>W0002</t>
+  </si>
+  <si>
+    <t>W0003</t>
+  </si>
+  <si>
+    <t>W0005</t>
+  </si>
+  <si>
+    <t>W0006</t>
+  </si>
+  <si>
+    <t>W0007</t>
+  </si>
+  <si>
+    <t>A0001</t>
+  </si>
+  <si>
+    <t>A0002</t>
+  </si>
+  <si>
+    <t>A0003</t>
+  </si>
+  <si>
+    <t>A0005</t>
+  </si>
+  <si>
+    <t>A0006</t>
+  </si>
+  <si>
+    <t>A0007</t>
   </si>
 </sst>
 </file>
@@ -83,13 +119,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -107,7 +150,7 @@
   <autoFilter ref="A2:C62" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="SummonGrade : Int"/>
-    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : Int"/>
+    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : String" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{6233F03A-7423-45FA-8858-E7CF6806ED7B}" name="Probability : Int"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -380,7 +423,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -397,21 +440,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>10001</v>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C3">
         <v>4995</v>
@@ -422,8 +465,8 @@
         <f>A3</f>
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>10002</v>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -434,8 +477,8 @@
         <f t="shared" ref="A5:A14" si="0">A4</f>
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>10003</v>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -446,8 +489,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B6">
-        <v>10005</v>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -458,8 +501,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>10006</v>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -470,8 +513,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B8">
-        <v>10007</v>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -482,8 +525,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B9">
-        <v>20001</v>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C9">
         <v>4995</v>
@@ -494,8 +537,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B10">
-        <v>20002</v>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -506,8 +549,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B11">
-        <v>20003</v>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -518,8 +561,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B12">
-        <v>20005</v>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -530,8 +573,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>20006</v>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -542,8 +585,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="B14">
-        <v>20007</v>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -557,9 +600,9 @@
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1" t="str">
         <f t="shared" ref="B15:B20" si="1">B3</f>
-        <v>10001</v>
+        <v>W0001</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -570,9 +613,9 @@
         <f>A15</f>
         <v>2</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10002</v>
+        <v>W0002</v>
       </c>
       <c r="C16">
         <v>4995</v>
@@ -583,9 +626,9 @@
         <f t="shared" ref="A17:A20" si="2">A16</f>
         <v>2</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10003</v>
+        <v>W0003</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -596,9 +639,9 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10005</v>
+        <v>W0005</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -609,9 +652,9 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10006</v>
+        <v>W0006</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -622,9 +665,9 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>10007</v>
+        <v>W0007</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -634,8 +677,8 @@
       <c r="A21">
         <v>2</v>
       </c>
-      <c r="B21">
-        <v>20001</v>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -646,8 +689,8 @@
         <f>A21</f>
         <v>2</v>
       </c>
-      <c r="B22">
-        <v>20002</v>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C22">
         <v>4995</v>
@@ -658,8 +701,8 @@
         <f t="shared" ref="A23:A26" si="3">A22</f>
         <v>2</v>
       </c>
-      <c r="B23">
-        <v>20003</v>
+      <c r="B23" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -670,8 +713,8 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="B24">
-        <v>20005</v>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -682,8 +725,8 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="B25">
-        <v>20006</v>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -694,8 +737,8 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="B26">
-        <v>20007</v>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -709,9 +752,9 @@
       <c r="A27">
         <v>3</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1" t="str">
         <f t="shared" ref="B27:B62" si="4">B15</f>
-        <v>10001</v>
+        <v>W0001</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -722,9 +765,9 @@
         <f>A27</f>
         <v>3</v>
       </c>
-      <c r="B28">
-        <f t="shared" si="4"/>
-        <v>10002</v>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -735,9 +778,9 @@
         <f t="shared" ref="A29:A32" si="5">A28</f>
         <v>3</v>
       </c>
-      <c r="B29">
-        <f t="shared" si="4"/>
-        <v>10003</v>
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
       </c>
       <c r="C29">
         <v>4995</v>
@@ -748,9 +791,9 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="B30">
-        <f t="shared" si="4"/>
-        <v>10005</v>
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -761,9 +804,9 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="4"/>
-        <v>10006</v>
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -774,9 +817,9 @@
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="4"/>
-        <v>10007</v>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -786,9 +829,9 @@
       <c r="A33">
         <v>3</v>
       </c>
-      <c r="B33">
-        <f t="shared" si="4"/>
-        <v>20001</v>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -799,9 +842,9 @@
         <f>A33</f>
         <v>3</v>
       </c>
-      <c r="B34">
-        <f t="shared" si="4"/>
-        <v>20002</v>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -812,9 +855,9 @@
         <f t="shared" ref="A35:A38" si="6">A34</f>
         <v>3</v>
       </c>
-      <c r="B35">
-        <f t="shared" si="4"/>
-        <v>20003</v>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
       </c>
       <c r="C35">
         <v>4995</v>
@@ -825,9 +868,9 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="B36">
-        <f t="shared" si="4"/>
-        <v>20005</v>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -838,9 +881,9 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="B37">
-        <f t="shared" si="4"/>
-        <v>20006</v>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -851,9 +894,9 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="B38">
-        <f t="shared" si="4"/>
-        <v>20007</v>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -863,9 +906,9 @@
       <c r="A39">
         <v>4</v>
       </c>
-      <c r="B39">
-        <f t="shared" si="4"/>
-        <v>10001</v>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -876,9 +919,9 @@
         <f>A39</f>
         <v>4</v>
       </c>
-      <c r="B40">
-        <f t="shared" si="4"/>
-        <v>10002</v>
+      <c r="B40" s="1" t="str">
+        <f>B28</f>
+        <v>W0002</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -889,9 +932,9 @@
         <f t="shared" ref="A41:A44" si="7">A40</f>
         <v>4</v>
       </c>
-      <c r="B41">
-        <f t="shared" si="4"/>
-        <v>10003</v>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -902,9 +945,9 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="B42">
-        <f t="shared" si="4"/>
-        <v>10005</v>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
       </c>
       <c r="C42">
         <v>4995</v>
@@ -915,9 +958,9 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="B43">
-        <f t="shared" si="4"/>
-        <v>10006</v>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -928,9 +971,9 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="B44">
-        <f t="shared" si="4"/>
-        <v>10007</v>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -940,9 +983,9 @@
       <c r="A45">
         <v>4</v>
       </c>
-      <c r="B45">
-        <f t="shared" si="4"/>
-        <v>20001</v>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -953,9 +996,9 @@
         <f>A45</f>
         <v>4</v>
       </c>
-      <c r="B46">
-        <f t="shared" si="4"/>
-        <v>20002</v>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -966,9 +1009,9 @@
         <f t="shared" ref="A47:A50" si="8">A46</f>
         <v>4</v>
       </c>
-      <c r="B47">
-        <f t="shared" si="4"/>
-        <v>20003</v>
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -979,9 +1022,9 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B48">
-        <f t="shared" si="4"/>
-        <v>20005</v>
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
       </c>
       <c r="C48">
         <v>4995</v>
@@ -992,9 +1035,9 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B49">
-        <f t="shared" si="4"/>
-        <v>20006</v>
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -1005,9 +1048,9 @@
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="B50">
-        <f t="shared" si="4"/>
-        <v>20007</v>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -1017,9 +1060,9 @@
       <c r="A51">
         <v>5</v>
       </c>
-      <c r="B51">
-        <f t="shared" si="4"/>
-        <v>10001</v>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -1030,9 +1073,9 @@
         <f>A51</f>
         <v>5</v>
       </c>
-      <c r="B52">
-        <f t="shared" si="4"/>
-        <v>10002</v>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -1043,9 +1086,9 @@
         <f t="shared" ref="A53:A56" si="9">A52</f>
         <v>5</v>
       </c>
-      <c r="B53">
-        <f t="shared" si="4"/>
-        <v>10003</v>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -1056,9 +1099,9 @@
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="B54">
-        <f t="shared" si="4"/>
-        <v>10005</v>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1069,9 +1112,9 @@
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="B55">
-        <f t="shared" si="4"/>
-        <v>10006</v>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
       </c>
       <c r="C55">
         <v>4995</v>
@@ -1082,9 +1125,9 @@
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="B56">
-        <f t="shared" si="4"/>
-        <v>10007</v>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1094,9 +1137,9 @@
       <c r="A57">
         <v>5</v>
       </c>
-      <c r="B57">
-        <f t="shared" si="4"/>
-        <v>20001</v>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -1107,9 +1150,9 @@
         <f>A57</f>
         <v>5</v>
       </c>
-      <c r="B58">
-        <f t="shared" si="4"/>
-        <v>20002</v>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1120,9 +1163,9 @@
         <f t="shared" ref="A59:A62" si="10">A58</f>
         <v>5</v>
       </c>
-      <c r="B59">
-        <f t="shared" si="4"/>
-        <v>20003</v>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -1133,9 +1176,9 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="B60">
-        <f t="shared" si="4"/>
-        <v>20005</v>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1146,9 +1189,9 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="B61">
-        <f t="shared" si="4"/>
-        <v>20006</v>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
       </c>
       <c r="C61">
         <v>4995</v>
@@ -1159,9 +1202,9 @@
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="B62">
-        <f t="shared" si="4"/>
-        <v>20007</v>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
       </c>
       <c r="C62">
         <v>1</v>

</xml_diff>

<commit_message>
[💡Feature] Summon type diversify work - 1
- 소환 배너 및 테이블 종류 추가 작업 베이스 추가
- SO 및 스크립트 추가
- (임시) 배경음 줄이기
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC36D6-CC60-48A7-A1C5-F664094E03AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9020F-0785-4191-B06F-4192576583D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Data\SummonTable\EquipmentSummonTable.json</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,6 +73,10 @@
   </si>
   <si>
     <t>A0007</t>
+  </si>
+  <si>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableEquipment.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -435,18 +435,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>4995</v>
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -490,7 +490,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -502,7 +502,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -514,7 +514,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>4995</v>
@@ -538,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -550,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -586,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -690,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>4995</v>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -714,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -726,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26">
         <v>1</v>

</xml_diff>

<commit_message>
[💡Feature] Summon type diversify work - 3
- 스킬, 동료 뽑기 테이블 추가 (json 변환 완료)
- 뽑기 버튼 기능 배너 프리팹으로 이관
- 팝업창은 뽑기 리스트의 배너 생성 및 초기화, 매니저 상호작용의 중간다리 역할
- UIBase.cs의 UI 로드 방식 임시 추가
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B9020F-0785-4191-B06F-4192576583D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5819316E-CF0A-49DB-B756-9E993049EE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Equipment" sheetId="1" r:id="rId1"/>
+    <sheet name="Skills" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
   <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +80,14 @@
     <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableEquipment.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableSkills.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableFollower.json</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -128,7 +138,13 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -150,8 +166,32 @@
   <autoFilter ref="A2:C62" xr:uid="{0E5758C5-4B07-4DCE-A258-64446AF4C7C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{33FA626A-A7BE-470D-B5F6-55BA5EC74483}" name="SummonGrade : Int"/>
-    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : String" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A1668163-0B67-492A-8817-4F251D1B8740}" name="ItemId : String" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{6233F03A-7423-45FA-8858-E7CF6806ED7B}" name="Probability : Int"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C62" totalsRowShown="0">
+  <autoFilter ref="A2:C62" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{06FEEBCF-143F-467A-94A3-ED6516C27AF9}" name="SummonGrade : Int"/>
+    <tableColumn id="2" xr3:uid="{94EF72E9-ADB9-4815-8659-1DBA16E8F4CA}" name="ItemId : String" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{04384F03-3803-4913-B128-0C0EC5B59BC8}" name="Probability : Int"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}" name="표1_34" displayName="표1_34" ref="A2:C62" totalsRowShown="0">
+  <autoFilter ref="A2:C62" xr:uid="{5A4DFF02-36B8-41E7-8806-3F9C3960FF2C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{33B2D4D5-FB6D-4D4D-BFB4-929061FDF8C7}" name="SummonGrade : Int"/>
+    <tableColumn id="2" xr3:uid="{ED56F630-FCAF-4415-A242-47AC6BE1C32C}" name="ItemId : String" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{6DBEC93B-2FF3-4A00-B929-EB47F158AC03}" name="Probability : Int"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -422,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1216,6 +1256,1609 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6FFAFD-B9D4-4D16-9C10-FE1E60CA3279}">
+  <dimension ref="A1:D62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A14" si="0">A4</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>SUM(C3:C14)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" ref="B15:B20" si="1">B3</f>
+        <v>W0001</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>A15</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0002</v>
+      </c>
+      <c r="C16">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" ref="A17:A20" si="2">A16</f>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0003</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0005</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0006</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0007</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>A21</f>
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" ref="A23:A26" si="3">A22</f>
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f>SUM(C15:C26)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" ref="B27:B62" si="4">B15</f>
+        <v>W0001</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f>A27</f>
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" ref="A29:A32" si="5">A28</f>
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C29">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>A33</f>
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" ref="A35:A38" si="6">A34</f>
+        <v>3</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C35">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f>A39</f>
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>B28</f>
+        <v>W0002</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" ref="A41:A44" si="7">A40</f>
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C42">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f>A45</f>
+        <v>4</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" ref="A47:A50" si="8">A46</f>
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C48">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f>A51</f>
+        <v>5</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" ref="A53:A56" si="9">A52</f>
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C55">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f>A57</f>
+        <v>5</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" ref="A59:A62" si="10">A58</f>
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C61">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1FBEA-E97D-46D7-B77D-7F9DD3257CDE}">
+  <dimension ref="A1:D62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="3" max="3" width="19.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>A3</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" ref="A5:A14" si="0">A4</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>SUM(C3:C14)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" ref="B15:B20" si="1">B3</f>
+        <v>W0001</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>A15</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0002</v>
+      </c>
+      <c r="C16">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" ref="A17:A20" si="2">A16</f>
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0003</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0005</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0006</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>W0007</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>A21</f>
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" ref="A23:A26" si="3">A22</f>
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f>SUM(C15:C26)</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1" t="str">
+        <f t="shared" ref="B27:B62" si="4">B15</f>
+        <v>W0001</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f>A27</f>
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" ref="A29:A32" si="5">A28</f>
+        <v>3</v>
+      </c>
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C29">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="B32" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f>A33</f>
+        <v>3</v>
+      </c>
+      <c r="B34" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" ref="A35:A38" si="6">A34</f>
+        <v>3</v>
+      </c>
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C35">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B37" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B38" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f>A39</f>
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="str">
+        <f>B28</f>
+        <v>W0002</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" ref="A41:A44" si="7">A40</f>
+        <v>4</v>
+      </c>
+      <c r="B41" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C42">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B43" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f>A45</f>
+        <v>4</v>
+      </c>
+      <c r="B46" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" ref="A47:A50" si="8">A46</f>
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C48">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0001</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f>A51</f>
+        <v>5</v>
+      </c>
+      <c r="B52" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0002</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" ref="A53:A56" si="9">A52</f>
+        <v>5</v>
+      </c>
+      <c r="B53" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0003</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B54" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0005</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B55" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0006</v>
+      </c>
+      <c r="C55">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B56" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>W0007</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0001</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f>A57</f>
+        <v>5</v>
+      </c>
+      <c r="B58" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0002</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" ref="A59:A62" si="10">A58</f>
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0003</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B60" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0005</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B61" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0006</v>
+      </c>
+      <c r="C61">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="B62" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>A0007</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[🛠️Fix] inventory type add
- 소환 시 타입별로 저장되는 인벤토리 구분하도록 스위치문으로 임시 추가
- 소환 데이터 변경
</commit_message>
<xml_diff>
--- a/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
+++ b/IdleGame/Assets/Resources/ExcelTable/SummonTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9834BC0D-C3B2-4F72-908C-68F2A9EF68D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C173C311-06D3-4DFE-AF63-B82FDFE0122A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="750" windowWidth="17205" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
   <si>
     <t>Probability : Int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,11 +81,30 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableSkills.json</t>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableFollower.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\SummonTableFollower.json</t>
+    <t>S0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S0002</t>
+  </si>
+  <si>
+    <t>S0003</t>
+  </si>
+  <si>
+    <t>S0004</t>
+  </si>
+  <si>
+    <t>S0005</t>
+  </si>
+  <si>
+    <t>S0006</t>
+  </si>
+  <si>
+    <t>D:\Project\TeamProject-IdleGame\IdleGame\Assets\Resources\Texts\Summon\SummonTableSkills.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -174,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C62" totalsRowShown="0">
-  <autoFilter ref="A2:C62" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}" name="표1_3" displayName="표1_3" ref="A2:C32" totalsRowShown="0">
+  <autoFilter ref="A2:C32" xr:uid="{EB499717-A1AC-43E5-BB07-2DDEA916DCA8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{06FEEBCF-143F-467A-94A3-ED6516C27AF9}" name="SummonGrade : Int"/>
     <tableColumn id="2" xr3:uid="{94EF72E9-ADB9-4815-8659-1DBA16E8F4CA}" name="ItemId : String" dataDxfId="1"/>
@@ -1262,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6FFAFD-B9D4-4D16-9C10-FE1E60CA3279}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1275,12 +1294,12 @@
     <col min="3" max="3" width="19.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1291,764 +1310,382 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A3</f>
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1996</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" ref="A5:A14" si="0">A4</f>
+        <f t="shared" ref="A5:A8" si="0">A4</f>
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f>B3</f>
+        <v>S0001</v>
       </c>
       <c r="C9">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
+        <f>A9</f>
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f>B4</f>
+        <v>S0002</v>
       </c>
       <c r="C10">
-        <v>1996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
+        <f t="shared" ref="A11:A14" si="1">A10</f>
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f>B5</f>
+        <v>S0003</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f>B6</f>
+        <v>S0004</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f>B7</f>
+        <v>S0005</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f>B8</f>
+        <v>S0006</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <f>SUM(C3:C14)</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="str">
-        <f t="shared" ref="B15:B20" si="1">B3</f>
-        <v>W0001</v>
+        <f>B9</f>
+        <v>S0001</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>A15</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>W0002</v>
+        <f>B10</f>
+        <v>S0002</v>
       </c>
       <c r="C16">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" ref="A17:A20" si="2">A16</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>W0003</v>
+        <f>B11</f>
+        <v>S0003</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>W0005</v>
+        <f>B12</f>
+        <v>S0004</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>W0006</v>
+        <f>B13</f>
+        <v>S0005</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>W0007</v>
+        <f>B14</f>
+        <v>S0006</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>B15</f>
+        <v>S0001</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>A21</f>
-        <v>2</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="str">
+        <f>B16</f>
+        <v>S0002</v>
       </c>
       <c r="C22">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" ref="A23:A26" si="3">A22</f>
-        <v>2</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="str">
+        <f>B17</f>
+        <v>S0003</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="str">
+        <f>B18</f>
+        <v>S0004</v>
       </c>
       <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>B19</f>
+        <v>S0005</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>B20</f>
+        <v>S0006</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26">
-        <f>SUM(C15:C26)</f>
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1" t="str">
-        <f t="shared" ref="B27:B62" si="4">B15</f>
-        <v>W0001</v>
+        <f>B21</f>
+        <v>S0001</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>A27</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B28" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0002</v>
+        <f>B22</f>
+        <v>S0002</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" ref="A29:A32" si="5">A28</f>
-        <v>3</v>
+        <f t="shared" ref="A29:A32" si="4">A28</f>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0003</v>
+        <f>B23</f>
+        <v>S0003</v>
       </c>
       <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="str">
+        <f>B24</f>
+        <v>S0004</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="str">
+        <f>B25</f>
+        <v>S0005</v>
+      </c>
+      <c r="C31">
         <v>4995</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="B30" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0005</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="B31" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0006</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="B32" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0007</v>
+        <f>B26</f>
+        <v>S0006</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>3</v>
-      </c>
-      <c r="B33" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0001</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f>A33</f>
-        <v>3</v>
-      </c>
-      <c r="B34" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0002</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <f t="shared" ref="A35:A38" si="6">A34</f>
-        <v>3</v>
-      </c>
-      <c r="B35" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0003</v>
-      </c>
-      <c r="C35">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="B36" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0005</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="B37" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0006</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="B38" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0007</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0001</v>
-      </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <f>A39</f>
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="str">
-        <f>B28</f>
-        <v>W0002</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" ref="A41:A44" si="7">A40</f>
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0003</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0005</v>
-      </c>
-      <c r="C42">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0006</v>
-      </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0007</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>4</v>
-      </c>
-      <c r="B45" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0001</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <f>A45</f>
-        <v>4</v>
-      </c>
-      <c r="B46" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0002</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <f t="shared" ref="A47:A50" si="8">A46</f>
-        <v>4</v>
-      </c>
-      <c r="B47" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0003</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="B48" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0005</v>
-      </c>
-      <c r="C48">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="B49" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0006</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="B50" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0007</v>
-      </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0001</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <f>A51</f>
-        <v>5</v>
-      </c>
-      <c r="B52" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0002</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53">
-        <f t="shared" ref="A53:A56" si="9">A52</f>
-        <v>5</v>
-      </c>
-      <c r="B53" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0003</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0005</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="B55" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0006</v>
-      </c>
-      <c r="C55">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <f t="shared" si="9"/>
-        <v>5</v>
-      </c>
-      <c r="B56" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>W0007</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0001</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f>A57</f>
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0002</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" ref="A59:A62" si="10">A58</f>
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0003</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="B60" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0005</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0006</v>
-      </c>
-      <c r="C61">
-        <v>4995</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="B62" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>A0007</v>
-      </c>
-      <c r="C62">
         <v>1</v>
       </c>
     </row>
@@ -2066,7 +1703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1FBEA-E97D-46D7-B77D-7F9DD3257CDE}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2079,7 +1716,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>